<commit_message>
fixed bug in Nt_c
</commit_message>
<xml_diff>
--- a/data_sets/Power/ODO_INPUT.xlsx
+++ b/data_sets/Power/ODO_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hlh/Dropbox/Work/Collaborations/Harsha/Networked_Microgrid/ODO/data_sets/Power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D7F1C-3C0D-A84D-9370-5CCF241F9991}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76BAD9C-EBF3-8144-8394-82801D7A9DBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" tabRatio="938" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9054" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9061" uniqueCount="370">
   <si>
     <t>January</t>
   </si>
@@ -1130,6 +1130,9 @@
     <t>branch_1_2</t>
   </si>
   <si>
+    <t>branch_2_3</t>
+  </si>
+  <si>
     <t>load_670a_phase_2</t>
   </si>
   <si>
@@ -1146,6 +1149,21 @@
   </si>
   <si>
     <t>nb hours (should be less than 288 hours = 12 days)</t>
+  </si>
+  <si>
+    <t>branch_7_8</t>
+  </si>
+  <si>
+    <t>branch_3_4</t>
+  </si>
+  <si>
+    <t>branch_6_16</t>
+  </si>
+  <si>
+    <t>branch_2_6</t>
+  </si>
+  <si>
+    <t>branch_2_7</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1503,6 +1521,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1686,7 +1710,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1713,6 +1737,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1760,7 +1785,47 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1881,6 +1946,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -1904,8 +1989,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
-      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2293,8 +2378,8 @@
   <sheetPr codeName="Sheet68"/>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4451,7 +4536,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9538,17 +9623,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="XFD5">
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:E36">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D18">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10505,18 +10590,21 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937DF613-129E-417F-876D-4B00A3A21EFA}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.83203125" bestFit="1" customWidth="1"/>
@@ -10526,20 +10614,20 @@
     <col min="26" max="27" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>362</v>
       </c>
       <c r="B2" s="19">
         <v>43466.25</v>
@@ -10556,14 +10644,45 @@
       <c r="F2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F2 D3:E3">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="D3:E3 D2">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10645,13 +10764,13 @@
         <v>350</v>
       </c>
       <c r="R1" t="s">
+        <v>360</v>
+      </c>
+      <c r="S1" t="s">
         <v>359</v>
       </c>
-      <c r="S1" t="s">
-        <v>358</v>
-      </c>
       <c r="T1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -31824,8 +31943,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I897"/>
   <sheetViews>
-    <sheetView zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A392" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="J395" sqref="J395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43256,10 +43375,10 @@
         <v>0</v>
       </c>
       <c r="G394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I394">
         <v>0</v>
@@ -43285,10 +43404,10 @@
         <v>0</v>
       </c>
       <c r="G395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I395">
         <v>0</v>
@@ -57854,7 +57973,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:I897">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59503,7 +59622,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:F81">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59516,7 +59635,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60603,12 +60722,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:U21 R2:U17">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61708,12 +61827,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:U21 R2:U17">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62086,7 +62205,7 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N3" sqref="A3:N3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -62152,7 +62271,7 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>6.5</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2">
         <v>6440</v>
@@ -62197,7 +62316,7 @@
         <v>41</v>
       </c>
       <c r="C3">
-        <v>7.5</v>
+        <v>75</v>
       </c>
       <c r="D3" s="2">
         <v>5761.407408</v>

</xml_diff>

<commit_message>
69 percent gap with/without networking
</commit_message>
<xml_diff>
--- a/data_sets/Power/ODO_INPUT.xlsx
+++ b/data_sets/Power/ODO_INPUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hlh/Dropbox/Work/Collaborations/Harsha/Networked_Microgrid/ODO/data_sets/Power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76BAD9C-EBF3-8144-8394-82801D7A9DBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E511DFEB-E5A6-4646-A187-F9CAAD118CF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" tabRatio="938" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2500" windowWidth="28800" windowHeight="16080" tabRatio="938" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RunSettings" sheetId="107" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9061" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9062" uniqueCount="372">
   <si>
     <t>January</t>
   </si>
@@ -1164,6 +1164,12 @@
   </si>
   <si>
     <t>branch_2_7</t>
+  </si>
+  <si>
+    <t>0,0,0,0,0,0,0,0,0</t>
+  </si>
+  <si>
+    <t>1e-5,0,0,0,1e-5,0,0,0,1e-5</t>
   </si>
 </sst>
 </file>
@@ -2379,7 +2385,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2448,19 +2454,19 @@
         <v>174</v>
       </c>
       <c r="C3" s="4">
-        <v>8500</v>
+        <v>850</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>314</v>
+        <v>370</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="F3">
-        <v>34.918144280588599</v>
-      </c>
-      <c r="G3" s="13">
-        <v>2</v>
+        <v>0.35</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>316</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -10592,7 +10598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937DF613-129E-417F-876D-4B00A3A21EFA}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -31943,8 +31949,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I897"/>
   <sheetViews>
-    <sheetView topLeftCell="A392" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
-      <selection activeCell="J395" sqref="J395"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="I226" sqref="I226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38503,10 +38509,10 @@
         <v>0</v>
       </c>
       <c r="G226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I226">
         <v>0</v>
@@ -38532,10 +38538,10 @@
         <v>0</v>
       </c>
       <c r="G227">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H227">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I227">
         <v>0</v>
@@ -43375,7 +43381,7 @@
         <v>0</v>
       </c>
       <c r="G394">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H394">
         <v>1</v>
@@ -43404,7 +43410,7 @@
         <v>0</v>
       </c>
       <c r="G395">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H395">
         <v>0</v>
@@ -43433,7 +43439,7 @@
         <v>0</v>
       </c>
       <c r="G396">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H396">
         <v>0</v>
@@ -44999,7 +45005,7 @@
         <v>0</v>
       </c>
       <c r="G450">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H450">
         <v>0</v>
@@ -45028,7 +45034,7 @@
         <v>0</v>
       </c>
       <c r="G451">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H451">
         <v>0</v>
@@ -45057,7 +45063,7 @@
         <v>0</v>
       </c>
       <c r="G452">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H452">
         <v>0</v>
@@ -62205,7 +62211,7 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -62271,10 +62277,10 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>65</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="2">
-        <v>6440</v>
+        <v>2000</v>
       </c>
       <c r="E2" s="1">
         <v>0.5</v>
@@ -62316,7 +62322,7 @@
         <v>41</v>
       </c>
       <c r="C3">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2">
         <v>5761.407408</v>

</xml_diff>